<commit_message>
working scanner, validating from excel
</commit_message>
<xml_diff>
--- a/backend/generated_student_data.xlsx
+++ b/backend/generated_student_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandogabrielle/Documents/Capstone/Attendance-Monitoring/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30008C5A-4E28-1C45-A72B-4F0898E5D865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96F72D-6B17-4549-8A43-63D7E577AD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new changes on qr scanner, integrated already to the frontend
</commit_message>
<xml_diff>
--- a/backend/generated_student_data.xlsx
+++ b/backend/generated_student_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandogabrielle/Documents/Capstone/Attendance-Monitoring/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96F72D-6B17-4549-8A43-63D7E577AD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0B051B-FBA0-9F42-B3F0-922669DF2389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>22-17-01</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>first_name</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Section A</t>
+  </si>
+  <si>
+    <t>Section B</t>
   </si>
 </sst>
 </file>
@@ -483,7 +492,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -506,13 +515,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -819,15 +842,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>141</v>
       </c>
@@ -837,8 +860,11 @@
       <c r="C1" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -848,8 +874,11 @@
       <c r="C2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -859,8 +888,11 @@
       <c r="C3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -870,8 +902,11 @@
       <c r="C4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -881,8 +916,11 @@
       <c r="C5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -892,8 +930,11 @@
       <c r="C6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -903,8 +944,11 @@
       <c r="C7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -914,8 +958,11 @@
       <c r="C8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -925,8 +972,11 @@
       <c r="C9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -936,8 +986,11 @@
       <c r="C10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -947,8 +1000,11 @@
       <c r="C11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -958,8 +1014,11 @@
       <c r="C12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -969,8 +1028,11 @@
       <c r="C13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -980,8 +1042,11 @@
       <c r="C14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -991,8 +1056,11 @@
       <c r="C15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1002,8 +1070,11 @@
       <c r="C16" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1013,8 +1084,11 @@
       <c r="C17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1024,8 +1098,11 @@
       <c r="C18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1035,8 +1112,11 @@
       <c r="C19" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1046,8 +1126,11 @@
       <c r="C20" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1057,8 +1140,11 @@
       <c r="C21" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1068,8 +1154,11 @@
       <c r="C22" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1079,8 +1168,11 @@
       <c r="C23" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1090,8 +1182,11 @@
       <c r="C24" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1101,8 +1196,11 @@
       <c r="C25" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1112,8 +1210,11 @@
       <c r="C26" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1123,8 +1224,11 @@
       <c r="C27" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1134,8 +1238,11 @@
       <c r="C28" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1145,8 +1252,11 @@
       <c r="C29" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1156,8 +1266,11 @@
       <c r="C30" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1167,8 +1280,11 @@
       <c r="C31" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1178,8 +1294,11 @@
       <c r="C32" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1189,8 +1308,11 @@
       <c r="C33" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1200,8 +1322,11 @@
       <c r="C34" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1211,8 +1336,11 @@
       <c r="C35" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1222,8 +1350,11 @@
       <c r="C36" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1233,8 +1364,11 @@
       <c r="C37" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1244,8 +1378,11 @@
       <c r="C38" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1255,8 +1392,11 @@
       <c r="C39" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1266,8 +1406,11 @@
       <c r="C40" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1277,8 +1420,11 @@
       <c r="C41" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1288,8 +1434,11 @@
       <c r="C42" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1299,8 +1448,11 @@
       <c r="C43" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1310,8 +1462,11 @@
       <c r="C44" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1321,8 +1476,11 @@
       <c r="C45" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1332,8 +1490,11 @@
       <c r="C46" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1343,8 +1504,11 @@
       <c r="C47" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1354,8 +1518,11 @@
       <c r="C48" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1365,8 +1532,11 @@
       <c r="C49" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1376,8 +1546,11 @@
       <c r="C50" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1386,6 +1559,9 @@
       </c>
       <c r="C51" t="s">
         <v>140</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>